<commit_message>
Update test results data - 2025-04-12 05:32 PM
Generated with VH Results Processing System

Processing completed:

- Processed IBA tests (Simple and Full)

- Processed FBS mock tests

- Generated optimized JSON files for Vercel deployment

- Updated students database

- Synced student emails from MongoDB

- Synced roleNumbers to MongoDB for FBS access
</commit_message>
<xml_diff>
--- a/Results/DU FBS Mocks/DU FBS Mock 7.xlsx
+++ b/Results/DU FBS Mocks/DU FBS Mock 7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VH Website\vh-website\Results\DU FBS Mocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FA15F5-10C2-4598-BFAF-519FAEF153B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CC27DC-A470-47FC-9BA1-ECFCAEDC205D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1236,8 +1236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:T4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1433,7 +1433,7 @@
       </c>
       <c r="Y2">
         <f t="shared" ref="Y2:Y26" si="12">_xlfn.RANK.EQ(X2, $X$2:$X$1002, 0)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Z2" s="19">
         <v>7</v>
@@ -1454,7 +1454,7 @@
       </c>
       <c r="AF2">
         <f t="shared" ref="AF2:AF26" si="14">_xlfn.RANK.EQ(AE2, $AE$2:$AE$1002, 0)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AG2" s="13"/>
       <c r="AH2">
@@ -1548,7 +1548,7 @@
       </c>
       <c r="Y3">
         <f t="shared" si="12"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Z3" s="20">
         <v>7.5</v>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="AF3">
         <f t="shared" si="14"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AG3" s="13"/>
       <c r="AH3">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="Y4">
         <f t="shared" si="12"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Z4" s="20">
         <v>7.5</v>
@@ -1684,7 +1684,7 @@
       </c>
       <c r="AF4">
         <f t="shared" si="14"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AG4" s="13"/>
       <c r="AH4">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="Y5">
         <f t="shared" si="12"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Z5" s="20">
         <v>6</v>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="AF5">
         <f t="shared" si="14"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AG5" s="13"/>
       <c r="AH5">
@@ -1914,7 +1914,7 @@
       </c>
       <c r="AF6">
         <f t="shared" si="14"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AH6">
         <f>SUM(AH1:AH5)</f>
@@ -2008,7 +2008,7 @@
       </c>
       <c r="Y7">
         <f t="shared" si="12"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Z7" s="20">
         <v>7</v>
@@ -2029,7 +2029,7 @@
       </c>
       <c r="AF7">
         <f t="shared" si="14"/>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -2089,7 +2089,7 @@
       </c>
       <c r="Y8">
         <f t="shared" si="12"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Z8" s="22"/>
       <c r="AA8" s="21"/>
@@ -2195,7 +2195,7 @@
       </c>
       <c r="Y9">
         <f t="shared" si="12"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Z9" s="19">
         <v>7</v>
@@ -2216,7 +2216,7 @@
       </c>
       <c r="AF9">
         <f t="shared" si="14"/>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -2276,7 +2276,7 @@
       </c>
       <c r="Y10">
         <f t="shared" si="12"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Z10" s="21"/>
       <c r="AA10" s="21"/>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="Y11">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Z11" s="20">
         <v>6</v>
@@ -2400,7 +2400,7 @@
       </c>
       <c r="AF11">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -2601,7 +2601,7 @@
       </c>
       <c r="Y13">
         <f t="shared" si="12"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Z13" s="19">
         <v>6.5</v>
@@ -2622,7 +2622,7 @@
       </c>
       <c r="AF13">
         <f t="shared" si="14"/>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -2793,7 +2793,7 @@
       </c>
       <c r="Y15">
         <f t="shared" si="12"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Z15" s="21"/>
       <c r="AA15" s="21"/>
@@ -2866,7 +2866,7 @@
       </c>
       <c r="Y16">
         <f t="shared" si="12"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Z16" s="21"/>
       <c r="AA16" s="21"/>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="Y17">
         <f t="shared" si="12"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Z17" s="21"/>
       <c r="AA17" s="21"/>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="Y18">
         <f t="shared" si="12"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Z18" s="21"/>
       <c r="AA18" s="21"/>
@@ -3196,7 +3196,7 @@
       </c>
       <c r="Y20">
         <f t="shared" si="12"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Z20" s="20">
         <v>6.5</v>
@@ -3307,7 +3307,7 @@
       </c>
       <c r="Y21">
         <f t="shared" si="12"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Z21" s="19">
         <v>7.5</v>
@@ -3328,7 +3328,7 @@
       </c>
       <c r="AF21">
         <f t="shared" si="14"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:32" ht="15" customHeight="1" thickBot="1">
@@ -3338,28 +3338,52 @@
       <c r="B22" s="6" t="s">
         <v>74</v>
       </c>
+      <c r="C22">
+        <v>14</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13.5</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>84.375</v>
+      </c>
+      <c r="G22">
+        <v>9</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
       </c>
       <c r="I22">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="J22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>70.833333333333343</v>
+      </c>
+      <c r="K22">
+        <v>14</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
       </c>
       <c r="M22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>13.5</v>
       </c>
       <c r="N22">
         <f t="shared" si="5"/>
+        <v>84.375</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
         <v>0</v>
       </c>
       <c r="Q22">
@@ -3370,25 +3394,31 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
+      <c r="S22">
+        <v>9</v>
+      </c>
+      <c r="T22">
+        <v>6</v>
+      </c>
       <c r="U22">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="V22">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>46.875</v>
       </c>
       <c r="W22">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="X22">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>71.666666666666671</v>
       </c>
       <c r="Y22">
         <f t="shared" si="12"/>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="Z22" s="23">
         <v>8.5</v>
@@ -3405,11 +3435,11 @@
       </c>
       <c r="AE22">
         <f t="shared" si="13"/>
-        <v>28.5</v>
+        <v>71.5</v>
       </c>
       <c r="AF22">
         <f t="shared" si="14"/>
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:32" ht="15" customHeight="1" thickBot="1">

</xml_diff>